<commit_message>
Ran tests on dijkstra's
</commit_message>
<xml_diff>
--- a/Data/Heapsort.xlsx
+++ b/Data/Heapsort.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AngusRitossa/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AngusRitossa/Desktop/Heaps/Heaps/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>2-ary</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Times are in milliseconds</t>
   </si>
 </sst>
 </file>
@@ -160,10 +163,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mj-lt"/>
                 <a:ea typeface="+mj-ea"/>
@@ -171,7 +171,11 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Heapsort</a:t>
             </a:r>
           </a:p>
@@ -193,10 +197,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mj-lt"/>
               <a:ea typeface="+mj-ea"/>
@@ -1681,11 +1682,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2085127072"/>
-        <c:axId val="-2109186496"/>
+        <c:axId val="2110834864"/>
+        <c:axId val="2110826656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2085127072"/>
+        <c:axId val="2110834864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1799,12 +1800,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2109186496"/>
+        <c:crossAx val="2110826656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2109186496"/>
+        <c:axId val="2110826656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1917,7 +1918,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2085127072"/>
+        <c:crossAx val="2110834864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2924,8 +2925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="94" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="134" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2945,6 +2946,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
       <c r="B1" s="1">
         <v>100000</v>
       </c>

</xml_diff>

<commit_message>
Ran tests on Edmond's algorithm
</commit_message>
<xml_diff>
--- a/Data/Heapsort.xlsx
+++ b/Data/Heapsort.xlsx
@@ -74,9 +74,6 @@
     <t>Pop</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Smooth forest</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>Times are in milliseconds</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -1682,11 +1682,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2110834864"/>
-        <c:axId val="2110826656"/>
+        <c:axId val="-2120643248"/>
+        <c:axId val="2115570512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2110834864"/>
+        <c:axId val="-2120643248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1800,12 +1800,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110826656"/>
+        <c:crossAx val="2115570512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2110826656"/>
+        <c:axId val="2115570512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1918,7 +1918,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110834864"/>
+        <c:crossAx val="-2120643248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2925,8 +2925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="134" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="134" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2947,7 +2947,7 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1">
         <v>100000</v>
@@ -3750,7 +3750,7 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>28</v>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>28</v>
@@ -4540,7 +4540,7 @@
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B36" s="1">
         <v>100000</v>
@@ -4836,7 +4836,7 @@
         <v>11171</v>
       </c>
       <c r="AA44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.2">

</xml_diff>